<commit_message>
added scrollDown utility, testLogger modified register test
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13940" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="63">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -41,21 +41,21 @@
     <t>verify the login test case</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>signinSignoutTest</t>
+  </si>
+  <si>
+    <t>newUserRegisterTest</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>signinSignoutTest</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>newUserRegisterTest</t>
-  </si>
-  <si>
     <t>TestName</t>
   </si>
   <si>
@@ -80,7 +80,16 @@
     <t>PhoneNo</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>RegisterPassword</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
   <si>
     <t>99123456</t>
@@ -116,10 +125,16 @@
     <t>1234</t>
   </si>
   <si>
-    <t>12345666</t>
-  </si>
-  <si>
-    <t>male</t>
+    <t>123445567</t>
+  </si>
+  <si>
+    <t>123456az</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
   <si>
     <t>12345690</t>
@@ -128,7 +143,7 @@
     <t>1235</t>
   </si>
   <si>
-    <t>12345667</t>
+    <t>123445568</t>
   </si>
   <si>
     <t>12345691</t>
@@ -137,7 +152,7 @@
     <t>1236</t>
   </si>
   <si>
-    <t>12345668</t>
+    <t>123445569</t>
   </si>
   <si>
     <t>12345692</t>
@@ -146,16 +161,7 @@
     <t>1237</t>
   </si>
   <si>
-    <t>12345669</t>
-  </si>
-  <si>
-    <t>12345693</t>
-  </si>
-  <si>
-    <t>1238</t>
-  </si>
-  <si>
-    <t>12345670</t>
+    <t>123445570</t>
   </si>
   <si>
     <t>12345694</t>
@@ -164,7 +170,7 @@
     <t>1239</t>
   </si>
   <si>
-    <t>12345671</t>
+    <t>123445572</t>
   </si>
   <si>
     <t>12345695</t>
@@ -173,7 +179,7 @@
     <t>1240</t>
   </si>
   <si>
-    <t>12345672</t>
+    <t>123445573</t>
   </si>
   <si>
     <t>12345696</t>
@@ -182,7 +188,7 @@
     <t>1241</t>
   </si>
   <si>
-    <t>12345673</t>
+    <t>123445574</t>
   </si>
   <si>
     <t>12345697</t>
@@ -191,7 +197,7 @@
     <t>1242</t>
   </si>
   <si>
-    <t>12345674</t>
+    <t>123445575</t>
   </si>
   <si>
     <t>12345698</t>
@@ -200,16 +206,7 @@
     <t>1243</t>
   </si>
   <si>
-    <t>12345675</t>
-  </si>
-  <si>
-    <t>12345699</t>
-  </si>
-  <si>
-    <t>1244</t>
-  </si>
-  <si>
-    <t>12345676</t>
+    <t>123445576</t>
   </si>
 </sst>
 </file>
@@ -897,12 +894,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -921,17 +921,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center"/>
@@ -1283,301 +1286,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="13" t="s">
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A6:A16">
+  <conditionalFormatting sqref="A10">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A9 A11:A15 A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1588,12 +1599,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1607,577 +1618,739 @@
     <col min="7" max="7" width="19.0078125" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.890625" style="2"/>
     <col min="9" max="9" width="14.4453125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.4921875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.890625" style="1"/>
+    <col min="10" max="10" width="16.6640625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="8.890625" style="3"/>
+    <col min="14" max="16384" width="8.890625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
+      <c r="K1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="E16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4">
-        <v>99123456</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>23</v>
+      <c r="D17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D16">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="A6:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1 A6:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A9 A11:A15 A17:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1 A6:A9 A11:A15 A17:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G7" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G8" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G9" r:id="rId1" display="sample@gmail.com"/>
-    <hyperlink ref="G10" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G11" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G12" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G13" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G14" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G15" r:id="rId1" display="sample@gmail.com"/>
-    <hyperlink ref="G16" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G17" r:id="rId1" display="NA"/>
+    <hyperlink ref="G16" r:id="rId1" display="NA"/>
+    <hyperlink ref="G10" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Added Language Preference test
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11860"/>
+    <workbookView windowWidth="28800" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$D$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$D$20</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="70">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -35,34 +35,43 @@
     <t>Priority</t>
   </si>
   <si>
+    <t>searchCategory</t>
+  </si>
+  <si>
+    <t>Searching the poroduct categorywise.</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>addProductToCart</t>
   </si>
   <si>
     <t>verify the login test case</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>signinSignoutTest</t>
   </si>
   <si>
-    <t>No</t>
+    <t>no</t>
   </si>
   <si>
     <t>newUserRegisterTest</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>searchCategory</t>
-  </si>
-  <si>
     <t>searchItem</t>
+  </si>
+  <si>
+    <t>Searching a particular Item.</t>
+  </si>
+  <si>
+    <t>languagePreference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecting lanaguage and verifying its impact. </t>
   </si>
   <si>
     <t>TestName</t>
@@ -226,9 +235,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -250,7 +259,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -258,25 +267,24 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -289,22 +297,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,8 +340,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,7 +395,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,58 +408,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -415,55 +424,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,127 +586,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,30 +672,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -698,15 +683,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,10 +704,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -740,8 +714,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -760,151 +734,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -921,10 +930,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1273,10 +1282,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1306,7 +1315,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1327,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1341,13 +1350,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>8</v>
@@ -1358,13 +1367,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>8</v>
@@ -1378,10 +1387,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>8</v>
@@ -1392,13 +1401,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>8</v>
@@ -1409,10 +1418,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -1426,10 +1435,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
@@ -1443,10 +1452,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>12</v>
@@ -1460,10 +1469,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>12</v>
@@ -1477,10 +1486,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>12</v>
@@ -1494,10 +1503,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -1511,10 +1520,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
@@ -1528,10 +1537,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>12</v>
@@ -1545,10 +1554,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>12</v>
@@ -1561,11 +1570,11 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="10" t="s">
-        <v>5</v>
+      <c r="A17" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>12</v>
@@ -1579,13 +1588,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>8</v>
@@ -1599,7 +1608,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
@@ -1611,13 +1620,33 @@
         <v>8</v>
       </c>
     </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A6:A16">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="A20">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+  <conditionalFormatting sqref="A7:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2 A18:A19 A21:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1628,12 +1657,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1653,34 +1682,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1691,28 +1720,28 @@
         <v>7</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1723,92 +1752,92 @@
         <v>7</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1816,86 +1845,86 @@
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>41</v>
@@ -1904,30 +1933,30 @@
         <v>42</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>44</v>
@@ -1936,30 +1965,30 @@
         <v>45</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>47</v>
@@ -1968,30 +1997,30 @@
         <v>48</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>50</v>
@@ -2000,30 +2029,30 @@
         <v>51</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>53</v>
@@ -2032,30 +2061,30 @@
         <v>54</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>56</v>
@@ -2064,30 +2093,30 @@
         <v>57</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>59</v>
@@ -2096,30 +2125,30 @@
         <v>60</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>62</v>
@@ -2128,30 +2157,30 @@
         <v>63</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>64</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>65</v>
@@ -2160,71 +2189,71 @@
         <v>66</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>24</v>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2235,42 +2264,75 @@
         <v>7</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D17">
+  <autoFilter ref="A1:D20">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="A6:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1 A6:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+  <conditionalFormatting sqref="A1:A2 A7:A19 A21:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G7" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G8" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G9" r:id="rId1" display="sample@gmail.com"/>
@@ -2281,9 +2343,11 @@
     <hyperlink ref="G14" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G15" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G16" r:id="rId1" display="sample@gmail.com"/>
-    <hyperlink ref="G17" r:id="rId1" display="NA"/>
+    <hyperlink ref="G17" r:id="rId1" display="sample@gmail.com"/>
     <hyperlink ref="G18" r:id="rId1" display="NA"/>
+    <hyperlink ref="G2" r:id="rId1" display="NA"/>
     <hyperlink ref="G19" r:id="rId1" display="NA"/>
+    <hyperlink ref="G20" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
refactored n config browserstack
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="97">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -185,12 +185,24 @@
     <t>13</t>
   </si>
   <si>
+    <t>placeOrderTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifying placing order </t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>TestName</t>
   </si>
   <si>
     <t>LoginCondition</t>
   </si>
   <si>
+    <t>LoginNeeded</t>
+  </si>
+  <si>
     <t>platformName</t>
   </si>
   <si>
@@ -257,10 +269,10 @@
     <t>emulator-5555</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>emulator-5556</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>emulator-5557</t>
@@ -1351,10 +1363,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1672,49 +1684,69 @@
         <v>54</v>
       </c>
     </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
     <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A10">
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A11">
     <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
+  <conditionalFormatting sqref="A13">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
+  <conditionalFormatting sqref="A14">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
+  <conditionalFormatting sqref="A15">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A16">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
+  <conditionalFormatting sqref="A17">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="A18">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="A19">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A19:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
+  <conditionalFormatting sqref="A1:A2 A20:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="23"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1725,1174 +1757,1296 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="26.1875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="2" customWidth="1"/>
-    <col min="5" max="6" width="21.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.9765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.4765625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.890625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="2" customWidth="1"/>
-    <col min="14" max="16" width="12.890625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.0078125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.890625" style="2"/>
-    <col min="19" max="16384" width="8.890625" style="1"/>
+    <col min="3" max="3" width="20.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.75" style="2" customWidth="1"/>
+    <col min="6" max="7" width="21.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.9765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.4765625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.890625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="12.890625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.0078125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.890625" style="2"/>
+    <col min="20" max="16384" width="8.890625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>74</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>77</v>
+      <c r="I4" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>77</v>
+      <c r="H5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H6" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H7" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H8" s="12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>76</v>
+      <c r="H9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H10" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H11" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H13" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H14" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H15" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H16" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R16" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H17" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H18" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R18" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>81</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="H19" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>77</v>
+      <c r="F20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17">
+  <autoFilter ref="A1:I17">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="A7">
+    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" dxfId="0" priority="25"/>
     <cfRule type="duplicateValues" dxfId="0" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
+  <conditionalFormatting sqref="A9">
     <cfRule type="duplicateValues" dxfId="0" priority="23"/>
     <cfRule type="duplicateValues" dxfId="0" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A10">
     <cfRule type="duplicateValues" dxfId="0" priority="21"/>
     <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A11:B11">
     <cfRule type="duplicateValues" dxfId="0" priority="19"/>
     <cfRule type="duplicateValues" dxfId="0" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:B11">
+  <conditionalFormatting sqref="A12:B12">
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:B12">
+  <conditionalFormatting sqref="A13:B13">
+    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
     <cfRule type="duplicateValues" dxfId="0" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:B13">
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B14">
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16">
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:B18">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:B19">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:B20">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B2 B3:B4 A5:A6 A20:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="41"/>
+  <conditionalFormatting sqref="A1:C2 B3:B4 A5:A6 A21:C1048576 C3:C20">
+    <cfRule type="duplicateValues" dxfId="0" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="43"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q5" r:id="rId1" display="sample@gmail.com"/>
-    <hyperlink ref="Q2" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q6" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q7" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q8" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q9" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q10" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q11" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q12" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q13" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q14" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q15" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q16" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q17" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q18" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q19" r:id="rId1" display="NA"/>
+    <hyperlink ref="R5" r:id="rId1" display="sample@gmail.com"/>
+    <hyperlink ref="R2" r:id="rId1" display="NA"/>
+    <hyperlink ref="R6" r:id="rId1" display="NA"/>
+    <hyperlink ref="R7" r:id="rId1" display="NA"/>
+    <hyperlink ref="R8" r:id="rId1" display="NA"/>
+    <hyperlink ref="R9" r:id="rId1" display="NA"/>
+    <hyperlink ref="R10" r:id="rId1" display="NA"/>
+    <hyperlink ref="R11" r:id="rId1" display="NA"/>
+    <hyperlink ref="R12" r:id="rId1" display="NA"/>
+    <hyperlink ref="R13" r:id="rId1" display="NA"/>
+    <hyperlink ref="R14" r:id="rId1" display="NA"/>
+    <hyperlink ref="R15" r:id="rId1" display="NA"/>
+    <hyperlink ref="R16" r:id="rId1" display="NA"/>
+    <hyperlink ref="R17" r:id="rId1" display="NA"/>
+    <hyperlink ref="R18" r:id="rId1" display="NA"/>
+    <hyperlink ref="R19" r:id="rId1" display="NA"/>
+    <hyperlink ref="R20" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Modified login functionality for tests
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$9</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="81">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -86,24 +86,21 @@
     <t>newUserRegisterTest</t>
   </si>
   <si>
-    <t>Searching a particular Item.</t>
+    <t>languagePreference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecting lanaguage and verifying its impact. </t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>changePasswordTest</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>languagePreference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selecting lanaguage and verifying its impact. </t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>changePasswordTest</t>
-  </si>
-  <si>
     <t>forgotPasswordTest</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
     <t>LoginCondition</t>
   </si>
   <si>
+    <t>LoginNeeded</t>
+  </si>
+  <si>
     <t>platformName</t>
   </si>
   <si>
@@ -191,6 +191,9 @@
     <t>userShouldLoggedIn</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Android</t>
   </si>
   <si>
@@ -212,6 +215,9 @@
     <t>emulator-5555</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>emulator-5556</t>
   </si>
   <si>
@@ -240,9 +246,6 @@
   </si>
   <si>
     <t>1234</t>
-  </si>
-  <si>
-    <t>emulator-5558</t>
   </si>
   <si>
     <t>emulator-5559</t>
@@ -1312,10 +1315,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1448,36 +1451,36 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1488,7 +1491,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
@@ -1505,7 +1508,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>8</v>
@@ -1519,24 +1522,24 @@
         <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
@@ -1545,15 +1548,15 @@
         <v>8</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>7</v>
@@ -1562,24 +1565,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1590,28 +1576,28 @@
     <cfRule type="duplicateValues" dxfId="0" priority="10"/>
     <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A9">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
+  <conditionalFormatting sqref="A10">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
+  <conditionalFormatting sqref="A11">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
+  <conditionalFormatting sqref="A12">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
+  <conditionalFormatting sqref="A13">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A14">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A8 A16:A1048576">
+  <conditionalFormatting sqref="A1:A2 A15:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,90 +1609,93 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="26.1875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="2" customWidth="1"/>
-    <col min="5" max="6" width="21.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.9765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.4765625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.890625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="2" customWidth="1"/>
-    <col min="14" max="16" width="12.890625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="19.0078125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.890625" style="2"/>
-    <col min="19" max="16384" width="8.890625" style="1"/>
+    <col min="1" max="3" width="26.1875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.75" style="2" customWidth="1"/>
+    <col min="6" max="7" width="21.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.9765625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.4765625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.890625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="12.890625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.0078125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="8.890625" style="2"/>
+    <col min="20" max="16384" width="8.890625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1714,15 +1703,15 @@
         <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -1731,38 +1720,41 @@
       <c r="H2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1770,16 +1762,16 @@
         <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>60</v>
@@ -1787,38 +1779,41 @@
       <c r="H3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1826,16 +1821,16 @@
         <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>60</v>
@@ -1843,111 +1838,117 @@
       <c r="H4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>60</v>
@@ -1955,55 +1956,58 @@
       <c r="H6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>60</v>
@@ -2011,166 +2015,175 @@
       <c r="H7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="12" t="s">
         <v>62</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>60</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>61</v>
+        <v>79</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="K8" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="L8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="J9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2179,54 +2192,57 @@
       <c r="H10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -2235,54 +2251,57 @@
       <c r="H11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G12" s="12" t="s">
@@ -2291,54 +2310,57 @@
       <c r="H12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G13" s="12" t="s">
@@ -2347,54 +2369,57 @@
       <c r="H13" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G14" s="12" t="s">
@@ -2403,150 +2428,96 @@
       <c r="H14" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="12" t="s">
         <v>62</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H10">
+  <autoFilter ref="A1:I9">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="A7">
+  <conditionalFormatting sqref="A6">
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
+  <conditionalFormatting sqref="A7">
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
     <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" dxfId="0" priority="13"/>
     <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A9">
     <cfRule type="duplicateValues" dxfId="0" priority="11"/>
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:B11">
+  <conditionalFormatting sqref="A10:B10">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
     <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A11:B11">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B14">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B2 B3:B4 A5:A6 A16:B1048576">
+  <conditionalFormatting sqref="A1:C2 B3:C4 A5 A15:C1048576 C5">
     <cfRule type="duplicateValues" dxfId="0" priority="30"/>
     <cfRule type="duplicateValues" dxfId="0" priority="33"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q5" r:id="rId1" display="sample@gmail.com"/>
-    <hyperlink ref="Q2" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q6" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q7" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q8" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q9" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q10" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q11" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q12" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q13" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q14" r:id="rId1" display="NA"/>
-    <hyperlink ref="Q15" r:id="rId1" display="NA"/>
+    <hyperlink ref="R5" r:id="rId1" display="sample@gmail.com"/>
+    <hyperlink ref="R2" r:id="rId1" display="NA"/>
+    <hyperlink ref="R6" r:id="rId1" display="NA"/>
+    <hyperlink ref="R7" r:id="rId1" display="NA"/>
+    <hyperlink ref="R8" r:id="rId1" display="NA"/>
+    <hyperlink ref="R9" r:id="rId1" display="NA"/>
+    <hyperlink ref="R10" r:id="rId1" display="NA"/>
+    <hyperlink ref="R11" r:id="rId1" display="NA"/>
+    <hyperlink ref="R12" r:id="rId1" display="NA"/>
+    <hyperlink ref="R13" r:id="rId1" display="NA"/>
+    <hyperlink ref="R14" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
test execution fix plus new tests added for add to cart module
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -4,21 +4,34 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11100" activeTab="1"/>
+    <workbookView windowWidth="25540" windowHeight="10780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$21</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="102">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -206,6 +219,21 @@
     <t>17</t>
   </si>
   <si>
+    <t>validateUserAddsNewPaymentMethod</t>
+  </si>
+  <si>
+    <t>Verifying user able to add card details</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>addToCartWithDifferentVariant</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>TestName</t>
   </si>
   <si>
@@ -279,6 +307,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>21177631</t>
   </si>
   <si>
     <t>12345689</t>
@@ -311,12 +342,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -351,16 +382,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,23 +421,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,6 +460,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -428,17 +484,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,38 +498,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,13 +533,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,13 +605,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,97 +689,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,49 +713,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,15 +781,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -770,6 +792,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,17 +844,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,175 +878,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1008,10 +1039,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,54 +1063,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1360,13 +1391,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="70" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.3359375" style="1" customWidth="1"/>
@@ -1715,52 +1746,94 @@
         <v>61</v>
       </c>
     </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
+  <conditionalFormatting sqref="A16">
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A19">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
+  <conditionalFormatting sqref="A20">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A21:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
+  <conditionalFormatting sqref="A1:A2 A23:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1771,15 +1844,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="2" width="26.1875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" style="2" customWidth="1"/>
@@ -1801,61 +1874,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1863,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1872,49 +1945,49 @@
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1922,7 +1995,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1931,49 +2004,49 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1981,58 +2054,58 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2040,58 +2113,58 @@
         <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2099,7 +2172,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2108,49 +2181,49 @@
         <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2158,7 +2231,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
@@ -2167,49 +2240,49 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2217,7 +2290,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -2226,49 +2299,49 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2276,58 +2349,58 @@
         <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -2335,7 +2408,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>7</v>
@@ -2344,49 +2417,49 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -2394,7 +2467,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
@@ -2403,49 +2476,49 @@
         <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2453,7 +2526,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>7</v>
@@ -2462,49 +2535,49 @@
         <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -2512,7 +2585,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
@@ -2521,49 +2594,49 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2571,7 +2644,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>7</v>
@@ -2580,49 +2653,49 @@
         <v>7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2630,7 +2703,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
@@ -2639,49 +2712,49 @@
         <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2689,7 +2762,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>7</v>
@@ -2698,49 +2771,49 @@
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -2748,7 +2821,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>7</v>
@@ -2757,49 +2830,49 @@
         <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -2807,7 +2880,7 @@
         <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>7</v>
@@ -2816,49 +2889,49 @@
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -2866,7 +2939,7 @@
         <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
@@ -2875,49 +2948,49 @@
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2925,7 +2998,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>7</v>
@@ -2934,118 +3007,252 @@
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>85</v>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I18">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I21" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="0" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:B11">
     <cfRule type="duplicateValues" dxfId="0" priority="33"/>
     <cfRule type="duplicateValues" dxfId="0" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A12:B12">
     <cfRule type="duplicateValues" dxfId="0" priority="31"/>
     <cfRule type="duplicateValues" dxfId="0" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A13:B13">
     <cfRule type="duplicateValues" dxfId="0" priority="29"/>
     <cfRule type="duplicateValues" dxfId="0" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:B11">
+  <conditionalFormatting sqref="A14:B14">
+    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B15">
     <cfRule type="duplicateValues" dxfId="0" priority="25"/>
     <cfRule type="duplicateValues" dxfId="0" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:B12">
+  <conditionalFormatting sqref="A16:B16">
     <cfRule type="duplicateValues" dxfId="0" priority="23"/>
     <cfRule type="duplicateValues" dxfId="0" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:B13">
+  <conditionalFormatting sqref="A17:B17">
     <cfRule type="duplicateValues" dxfId="0" priority="21"/>
     <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:B14">
+  <conditionalFormatting sqref="A18:B18">
     <cfRule type="duplicateValues" dxfId="0" priority="19"/>
     <cfRule type="duplicateValues" dxfId="0" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16:B16">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B17">
+  <conditionalFormatting sqref="A19:B19">
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="duplicateValues" dxfId="0" priority="13"/>
     <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B18">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:B19">
+  <conditionalFormatting sqref="B20:C20">
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:C20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C2 B3:C4 A5:A6 A21:C1048576 C5:C18">
-    <cfRule type="duplicateValues" dxfId="0" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C2 B3:C4 A5:A6 A21:A22 A23:C1048576 C5:C18">
+    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="59"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" display="sample@gmail.com"/>
@@ -3064,6 +3271,8 @@
     <hyperlink ref="R17" r:id="rId1" display="NA"/>
     <hyperlink ref="R18" r:id="rId1" display="NA"/>
     <hyperlink ref="R19" r:id="rId1" display="NA"/>
+    <hyperlink ref="R21" r:id="rId1" display="NA"/>
+    <hyperlink ref="R22" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
test fixed and new test added
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/MobileTestData.xlsx
+++ b/src/main/resources/excelFiles/MobileTestData.xlsx
@@ -4,21 +4,34 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11100" activeTab="1"/>
+    <workbookView windowWidth="25540" windowHeight="11360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$I$22</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="103">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -206,6 +219,24 @@
     <t>17</t>
   </si>
   <si>
+    <t>addToCartWithDifferentVariant</t>
+  </si>
+  <si>
+    <t>Verifying user able to add item selecting different variant</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>differentVariantsAddedSeparately</t>
+  </si>
+  <si>
+    <t>Verify different variants added separately in cart</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>TestName</t>
   </si>
   <si>
@@ -279,6 +310,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>21177631</t>
   </si>
   <si>
     <t>12345689</t>
@@ -311,12 +345,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -351,16 +385,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,23 +424,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,6 +463,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -428,17 +487,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,38 +501,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,13 +536,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,13 +608,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,97 +692,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,49 +716,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,15 +784,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -770,6 +795,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,17 +847,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,175 +881,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1008,10 +1042,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,54 +1066,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1360,13 +1394,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="70" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.3359375" style="1" customWidth="1"/>
@@ -1715,52 +1749,86 @@
         <v>61</v>
       </c>
     </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
+  <conditionalFormatting sqref="A16">
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A19">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A21:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
+  <conditionalFormatting sqref="A20:A22">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2 A23:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1771,17 +1839,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="$A22:$XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="2" width="26.1875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1875" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="2" customWidth="1"/>
@@ -1801,61 +1870,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1863,7 +1932,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1872,49 +1941,49 @@
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1922,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1931,49 +2000,49 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1981,58 +2050,58 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2040,58 +2109,58 @@
         <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2099,7 +2168,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2108,49 +2177,49 @@
         <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2158,7 +2227,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
@@ -2167,49 +2236,49 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2217,7 +2286,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -2226,49 +2295,49 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2276,58 +2345,58 @@
         <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -2335,7 +2404,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>7</v>
@@ -2344,49 +2413,49 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -2394,7 +2463,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
@@ -2403,49 +2472,49 @@
         <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2453,7 +2522,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>7</v>
@@ -2462,49 +2531,49 @@
         <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -2512,7 +2581,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
@@ -2521,49 +2590,49 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2571,7 +2640,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>7</v>
@@ -2580,49 +2649,49 @@
         <v>7</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2630,7 +2699,7 @@
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>7</v>
@@ -2639,49 +2708,49 @@
         <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2689,7 +2758,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>7</v>
@@ -2698,49 +2767,49 @@
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -2748,7 +2817,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>7</v>
@@ -2757,49 +2826,49 @@
         <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -2807,7 +2876,7 @@
         <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>7</v>
@@ -2816,49 +2885,49 @@
         <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -2866,7 +2935,7 @@
         <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>7</v>
@@ -2875,49 +2944,49 @@
         <v>7</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2925,7 +2994,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>7</v>
@@ -2934,118 +3003,252 @@
         <v>7</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>58</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I18">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I22" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="A7">
+    <cfRule type="duplicateValues" dxfId="0" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="duplicateValues" dxfId="0" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:B11">
+    <cfRule type="duplicateValues" dxfId="0" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:B12">
+    <cfRule type="duplicateValues" dxfId="0" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:B13">
+    <cfRule type="duplicateValues" dxfId="0" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:B14">
     <cfRule type="duplicateValues" dxfId="0" priority="35"/>
     <cfRule type="duplicateValues" dxfId="0" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
+  <conditionalFormatting sqref="A15:B15">
     <cfRule type="duplicateValues" dxfId="0" priority="33"/>
     <cfRule type="duplicateValues" dxfId="0" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A16:B16">
     <cfRule type="duplicateValues" dxfId="0" priority="31"/>
     <cfRule type="duplicateValues" dxfId="0" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
+  <conditionalFormatting sqref="A17:B17">
     <cfRule type="duplicateValues" dxfId="0" priority="29"/>
     <cfRule type="duplicateValues" dxfId="0" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:B11">
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:B12">
-    <cfRule type="duplicateValues" dxfId="0" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:B13">
+  <conditionalFormatting sqref="A18:B18">
+    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:B19">
+    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="duplicateValues" dxfId="0" priority="21"/>
     <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:B14">
-    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B15">
+  <conditionalFormatting sqref="B20:C20">
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:B16">
-    <cfRule type="duplicateValues" dxfId="0" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B17">
-    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18:B18">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:B19">
+  <conditionalFormatting sqref="B21">
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:C20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C2 B3:C4 A5:A6 A21:C1048576 C5:C18">
-    <cfRule type="duplicateValues" dxfId="0" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C2 B3:C4 A5:A6 C5:C18 A23:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="67"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="R5" r:id="rId1" display="sample@gmail.com"/>
@@ -3064,6 +3267,8 @@
     <hyperlink ref="R17" r:id="rId1" display="NA"/>
     <hyperlink ref="R18" r:id="rId1" display="NA"/>
     <hyperlink ref="R19" r:id="rId1" display="NA"/>
+    <hyperlink ref="R21" r:id="rId1" display="NA"/>
+    <hyperlink ref="R22" r:id="rId1" display="NA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>